<commit_message>
upload all coefficents for each leg
</commit_message>
<xml_diff>
--- a/save_coefficent/servo_DEG-PWM.xlsx
+++ b/save_coefficent/servo_DEG-PWM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\OneDrive\Desktop\1semestre\Bonzo - GoodBoy 0.0.0\botzo_v2s_github\calibrate_servos\save_coefficent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E712CA-5F9E-4D33-A163-C703910C0224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607681BE-8079-4854-BB4A-FC4EE6317877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
   <si>
     <t>DATASHEET</t>
   </si>
@@ -93,6 +93,42 @@
   </si>
   <si>
     <t>FRONT RIGHT</t>
+  </si>
+  <si>
+    <t>FRONT LEFT</t>
+  </si>
+  <si>
+    <t>SFL</t>
+  </si>
+  <si>
+    <t>FFL</t>
+  </si>
+  <si>
+    <t>TFL</t>
+  </si>
+  <si>
+    <t>BACK RIGHT</t>
+  </si>
+  <si>
+    <t>SBR</t>
+  </si>
+  <si>
+    <t>FBR</t>
+  </si>
+  <si>
+    <t>TBR</t>
+  </si>
+  <si>
+    <t>SBL</t>
+  </si>
+  <si>
+    <t>BACK LEFT</t>
+  </si>
+  <si>
+    <t>FBL</t>
+  </si>
+  <si>
+    <t>TBL</t>
   </si>
 </sst>
 </file>
@@ -362,6 +398,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -382,9 +421,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,8 +641,8 @@
   </sheetPr>
   <dimension ref="B5:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="63" workbookViewId="0">
+      <selection activeCell="L95" sqref="L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -683,31 +719,31 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="16"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="18" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
       <c r="H18" s="9" t="s">
         <v>7</v>
       </c>
@@ -739,7 +775,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="3">
@@ -755,18 +791,18 @@
         <f>E20-D20</f>
         <v>64</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="21">
         <v>1E-3</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="21">
         <v>7.2309999999999999</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="21">
         <v>563.08500000000004</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="3">
         <v>45</v>
       </c>
@@ -780,12 +816,12 @@
         <f t="shared" ref="F21:F34" si="0">E21-D21</f>
         <v>57</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="25"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="3">
         <v>90</v>
       </c>
@@ -799,12 +835,12 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="3">
         <v>135</v>
       </c>
@@ -818,12 +854,12 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="26"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="5">
         <v>180</v>
       </c>
@@ -833,16 +869,16 @@
       <c r="E24" s="5">
         <v>1897</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="15">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="3">
@@ -854,22 +890,22 @@
       <c r="E25" s="3">
         <v>606</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="16">
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="21">
         <v>0</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="21">
         <v>7.3479999999999999</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="21">
         <v>603.45699999999999</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="25"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="3">
         <v>45</v>
       </c>
@@ -883,12 +919,12 @@
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="3">
         <v>90</v>
       </c>
@@ -902,12 +938,12 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="3">
         <v>135</v>
       </c>
@@ -921,12 +957,12 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="26"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="5">
         <v>180</v>
       </c>
@@ -936,16 +972,16 @@
       <c r="E29" s="5">
         <v>1930</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="15">
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="3">
@@ -957,22 +993,22 @@
       <c r="E30" s="3">
         <v>555</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="16">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="21">
         <v>0</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="21">
         <v>7.5759999999999996</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="21">
         <v>554.28499999999997</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="25"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="3">
         <v>45</v>
       </c>
@@ -986,12 +1022,12 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="25"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="3">
         <v>90</v>
       </c>
@@ -1005,12 +1041,12 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="25"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="3">
         <v>135</v>
       </c>
@@ -1024,12 +1060,12 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="5">
         <v>180</v>
       </c>
@@ -1043,27 +1079,27 @@
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
-      <c r="F35" s="29"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="39" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
     </row>
     <row r="40" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="23"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="26"/>
       <c r="H40" s="9" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1131,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="3">
@@ -1111,12 +1147,18 @@
         <f>E42-D42</f>
         <v>100</v>
       </c>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
+      <c r="H42" s="21">
+        <v>0</v>
+      </c>
+      <c r="I42" s="21">
+        <v>7.5270000000000001</v>
+      </c>
+      <c r="J42" s="21">
+        <v>597.6</v>
+      </c>
     </row>
     <row r="43" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="25"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="3">
         <v>45</v>
       </c>
@@ -1130,12 +1172,12 @@
         <f t="shared" ref="F43:F56" si="1">E43-D43</f>
         <v>100</v>
       </c>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="25"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="3">
         <v>90</v>
       </c>
@@ -1149,12 +1191,12 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="3">
         <v>135</v>
       </c>
@@ -1168,12 +1210,12 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="5">
         <v>180</v>
       </c>
@@ -1183,16 +1225,16 @@
       <c r="E46" s="5">
         <v>1940</v>
       </c>
-      <c r="F46" s="27">
+      <c r="F46" s="15">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
     </row>
     <row r="47" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C47" s="3">
@@ -1204,16 +1246,22 @@
       <c r="E47" s="3">
         <v>580</v>
       </c>
-      <c r="F47" s="28">
+      <c r="F47" s="16">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="21">
+        <v>0</v>
+      </c>
+      <c r="I47" s="21">
+        <v>7.6820000000000004</v>
+      </c>
+      <c r="J47" s="21">
+        <v>578.14200000000005</v>
+      </c>
     </row>
     <row r="48" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="25"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="3">
         <v>45</v>
       </c>
@@ -1227,12 +1275,12 @@
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
     </row>
     <row r="49" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="25"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="3">
         <v>90</v>
       </c>
@@ -1246,12 +1294,12 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
     </row>
     <row r="50" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B50" s="25"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="3">
         <v>135</v>
       </c>
@@ -1265,12 +1313,12 @@
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
     </row>
     <row r="51" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="26"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="5">
         <v>180</v>
       </c>
@@ -1280,16 +1328,16 @@
       <c r="E51" s="5">
         <v>1935</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="15">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
     </row>
     <row r="52" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="3">
@@ -1301,16 +1349,22 @@
       <c r="E52" s="3">
         <v>620</v>
       </c>
-      <c r="F52" s="28">
+      <c r="F52" s="16">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
+      <c r="H52" s="21">
+        <v>0</v>
+      </c>
+      <c r="I52" s="21">
+        <v>7.3140000000000001</v>
+      </c>
+      <c r="J52" s="21">
+        <v>619.02800000000002</v>
+      </c>
     </row>
     <row r="53" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="25"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="3">
         <v>45</v>
       </c>
@@ -1324,12 +1378,12 @@
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
     </row>
     <row r="54" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="25"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="3">
         <v>90</v>
       </c>
@@ -1343,12 +1397,12 @@
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
     </row>
     <row r="55" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B55" s="25"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="3">
         <v>135</v>
       </c>
@@ -1362,12 +1416,12 @@
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
     </row>
     <row r="56" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="26"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="5">
         <v>180</v>
       </c>
@@ -1381,14 +1435,14 @@
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
     </row>
     <row r="57" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
-      <c r="F57" s="29"/>
+      <c r="F57" s="17"/>
     </row>
     <row r="58" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C58" s="12"/>
@@ -1411,11 +1465,13 @@
       <c r="D62" s="12"/>
     </row>
     <row r="63" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="21"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="23"/>
+      <c r="B63" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="26"/>
       <c r="H63" s="9" t="s">
         <v>7</v>
       </c>
@@ -1447,8 +1503,8 @@
       </c>
     </row>
     <row r="65" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B65" s="24" t="s">
-        <v>15</v>
+      <c r="B65" s="27" t="s">
+        <v>21</v>
       </c>
       <c r="C65" s="3">
         <v>0</v>
@@ -1456,86 +1512,102 @@
       <c r="D65" s="12">
         <v>500</v>
       </c>
-      <c r="E65" s="3"/>
+      <c r="E65" s="3">
+        <v>590</v>
+      </c>
       <c r="F65" s="13">
         <f>E65-D65</f>
-        <v>-500</v>
-      </c>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="18"/>
+        <v>90</v>
+      </c>
+      <c r="H65" s="21">
+        <v>0</v>
+      </c>
+      <c r="I65" s="21">
+        <v>7.4930000000000003</v>
+      </c>
+      <c r="J65" s="21">
+        <v>588.14200000000005</v>
+      </c>
     </row>
     <row r="66" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B66" s="25"/>
+      <c r="B66" s="28"/>
       <c r="C66" s="3">
         <v>45</v>
       </c>
       <c r="D66" s="12">
         <v>833</v>
       </c>
-      <c r="E66" s="3"/>
+      <c r="E66" s="3">
+        <v>925</v>
+      </c>
       <c r="F66" s="13">
         <f t="shared" ref="F66:F79" si="2">E66-D66</f>
-        <v>-833</v>
-      </c>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
+        <v>92</v>
+      </c>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
     </row>
     <row r="67" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B67" s="25"/>
+      <c r="B67" s="28"/>
       <c r="C67" s="3">
         <v>90</v>
       </c>
       <c r="D67" s="12">
         <v>1167</v>
       </c>
-      <c r="E67" s="3"/>
+      <c r="E67" s="3">
+        <v>1260</v>
+      </c>
       <c r="F67" s="13">
         <f t="shared" si="2"/>
-        <v>-1167</v>
-      </c>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
+        <v>93</v>
+      </c>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
     </row>
     <row r="68" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B68" s="25"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="3">
         <v>135</v>
       </c>
       <c r="D68" s="12">
         <v>1500</v>
       </c>
-      <c r="E68" s="3"/>
+      <c r="E68" s="3">
+        <v>1620</v>
+      </c>
       <c r="F68" s="13">
         <f t="shared" si="2"/>
-        <v>-1500</v>
-      </c>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
+        <v>120</v>
+      </c>
+      <c r="H68" s="22"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
     </row>
     <row r="69" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="26"/>
+      <c r="B69" s="29"/>
       <c r="C69" s="5">
         <v>180</v>
       </c>
       <c r="D69" s="14">
         <v>1833</v>
       </c>
-      <c r="E69" s="5"/>
-      <c r="F69" s="27">
+      <c r="E69" s="5">
+        <v>1950</v>
+      </c>
+      <c r="F69" s="15">
         <f t="shared" si="2"/>
-        <v>-1833</v>
-      </c>
-      <c r="H69" s="20"/>
-      <c r="I69" s="20"/>
-      <c r="J69" s="20"/>
+        <v>117</v>
+      </c>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
     </row>
     <row r="70" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="24" t="s">
-        <v>16</v>
+      <c r="B70" s="27" t="s">
+        <v>22</v>
       </c>
       <c r="C70" s="3">
         <v>0</v>
@@ -1543,86 +1615,102 @@
       <c r="D70" s="12">
         <v>500</v>
       </c>
-      <c r="E70" s="3"/>
-      <c r="F70" s="28">
+      <c r="E70" s="3">
+        <v>630</v>
+      </c>
+      <c r="F70" s="16">
         <f t="shared" si="2"/>
-        <v>-500</v>
-      </c>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="18"/>
+        <v>130</v>
+      </c>
+      <c r="H70" s="21">
+        <v>0</v>
+      </c>
+      <c r="I70" s="21">
+        <v>7.6029999999999998</v>
+      </c>
+      <c r="J70" s="21">
+        <v>625.428</v>
+      </c>
     </row>
     <row r="71" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="25"/>
+      <c r="B71" s="28"/>
       <c r="C71" s="3">
         <v>45</v>
       </c>
       <c r="D71" s="12">
         <v>833</v>
       </c>
-      <c r="E71" s="3"/>
+      <c r="E71" s="3">
+        <v>960</v>
+      </c>
       <c r="F71" s="13">
         <f t="shared" si="2"/>
-        <v>-833</v>
-      </c>
-      <c r="H71" s="19"/>
-      <c r="I71" s="19"/>
-      <c r="J71" s="19"/>
+        <v>127</v>
+      </c>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="22"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="25"/>
+      <c r="B72" s="28"/>
       <c r="C72" s="3">
         <v>90</v>
       </c>
       <c r="D72" s="12">
         <v>1167</v>
       </c>
-      <c r="E72" s="3"/>
+      <c r="E72" s="3">
+        <v>1310</v>
+      </c>
       <c r="F72" s="13">
         <f t="shared" si="2"/>
-        <v>-1167</v>
-      </c>
-      <c r="H72" s="19"/>
-      <c r="I72" s="19"/>
-      <c r="J72" s="19"/>
+        <v>143</v>
+      </c>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="25"/>
+      <c r="B73" s="28"/>
       <c r="C73" s="3">
         <v>135</v>
       </c>
       <c r="D73" s="12">
         <v>1500</v>
       </c>
-      <c r="E73" s="3"/>
+      <c r="E73" s="3">
+        <v>1670</v>
+      </c>
       <c r="F73" s="13">
         <f t="shared" si="2"/>
-        <v>-1500</v>
-      </c>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
-      <c r="J73" s="19"/>
+        <v>170</v>
+      </c>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="26"/>
+      <c r="B74" s="29"/>
       <c r="C74" s="5">
         <v>180</v>
       </c>
       <c r="D74" s="14">
         <v>1833</v>
       </c>
-      <c r="E74" s="5"/>
-      <c r="F74" s="27">
+      <c r="E74" s="5">
+        <v>2000</v>
+      </c>
+      <c r="F74" s="15">
         <f t="shared" si="2"/>
-        <v>-1833</v>
-      </c>
-      <c r="H74" s="20"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="20"/>
+        <v>167</v>
+      </c>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+      <c r="J74" s="23"/>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="24" t="s">
-        <v>17</v>
+      <c r="B75" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="C75" s="3">
         <v>0</v>
@@ -1630,93 +1718,111 @@
       <c r="D75" s="12">
         <v>500</v>
       </c>
-      <c r="E75" s="3"/>
-      <c r="F75" s="28">
+      <c r="E75" s="3">
+        <v>550</v>
+      </c>
+      <c r="F75" s="16">
         <f t="shared" si="2"/>
-        <v>-500</v>
-      </c>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="H75" s="21">
+        <v>1E-3</v>
+      </c>
+      <c r="I75" s="21">
+        <v>7.2329999999999997</v>
+      </c>
+      <c r="J75" s="21">
+        <v>549.99900000000002</v>
+      </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="25"/>
+      <c r="B76" s="28"/>
       <c r="C76" s="3">
         <v>45</v>
       </c>
       <c r="D76" s="12">
         <v>833</v>
       </c>
-      <c r="E76" s="3"/>
+      <c r="E76" s="3">
+        <v>880</v>
+      </c>
       <c r="F76" s="13">
         <f t="shared" si="2"/>
-        <v>-833</v>
-      </c>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="19"/>
+        <v>47</v>
+      </c>
+      <c r="H76" s="22"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="25"/>
+      <c r="B77" s="28"/>
       <c r="C77" s="3">
         <v>90</v>
       </c>
       <c r="D77" s="12">
         <v>1167</v>
       </c>
-      <c r="E77" s="3"/>
+      <c r="E77" s="3">
+        <v>1205</v>
+      </c>
       <c r="F77" s="13">
         <f t="shared" si="2"/>
-        <v>-1167</v>
-      </c>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
-      <c r="J77" s="19"/>
+        <v>38</v>
+      </c>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="25"/>
+      <c r="B78" s="28"/>
       <c r="C78" s="3">
         <v>135</v>
       </c>
       <c r="D78" s="12">
         <v>1500</v>
       </c>
-      <c r="E78" s="3"/>
+      <c r="E78" s="3">
+        <v>1555</v>
+      </c>
       <c r="F78" s="13">
         <f t="shared" si="2"/>
-        <v>-1500</v>
-      </c>
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
-      <c r="J78" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="H78" s="22"/>
+      <c r="I78" s="22"/>
+      <c r="J78" s="22"/>
     </row>
     <row r="79" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="26"/>
+      <c r="B79" s="29"/>
       <c r="C79" s="5">
         <v>180</v>
       </c>
       <c r="D79" s="14">
         <v>1833</v>
       </c>
-      <c r="E79" s="5"/>
+      <c r="E79" s="5">
+        <v>1890</v>
+      </c>
       <c r="F79" s="13">
         <f t="shared" si="2"/>
-        <v>-1833</v>
-      </c>
-      <c r="H79" s="20"/>
-      <c r="I79" s="20"/>
-      <c r="J79" s="20"/>
+        <v>57</v>
+      </c>
+      <c r="H79" s="23"/>
+      <c r="I79" s="23"/>
+      <c r="J79" s="23"/>
     </row>
     <row r="80" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F80" s="29"/>
+      <c r="F80" s="17"/>
     </row>
     <row r="84" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="21"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="23"/>
+      <c r="B85" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="26"/>
       <c r="H85" s="9" t="s">
         <v>7</v>
       </c>
@@ -1748,8 +1854,8 @@
       </c>
     </row>
     <row r="87" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="24" t="s">
-        <v>15</v>
+      <c r="B87" s="27" t="s">
+        <v>25</v>
       </c>
       <c r="C87" s="3">
         <v>0</v>
@@ -1757,86 +1863,102 @@
       <c r="D87" s="12">
         <v>500</v>
       </c>
-      <c r="E87" s="3"/>
+      <c r="E87" s="3">
+        <v>590</v>
+      </c>
       <c r="F87" s="13">
         <f>E87-D87</f>
-        <v>-500</v>
-      </c>
-      <c r="H87" s="18"/>
-      <c r="I87" s="18"/>
-      <c r="J87" s="18"/>
+        <v>90</v>
+      </c>
+      <c r="H87" s="21">
+        <v>1E-3</v>
+      </c>
+      <c r="I87" s="21">
+        <v>7.3869999999999996</v>
+      </c>
+      <c r="J87" s="21">
+        <v>584.28499999999997</v>
+      </c>
     </row>
     <row r="88" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="25"/>
+      <c r="B88" s="28"/>
       <c r="C88" s="3">
         <v>45</v>
       </c>
       <c r="D88" s="12">
         <v>833</v>
       </c>
-      <c r="E88" s="3"/>
+      <c r="E88" s="3">
+        <v>910</v>
+      </c>
       <c r="F88" s="13">
         <f t="shared" ref="F88:F101" si="3">E88-D88</f>
-        <v>-833</v>
-      </c>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
-      <c r="J88" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="H88" s="22"/>
+      <c r="I88" s="22"/>
+      <c r="J88" s="22"/>
     </row>
     <row r="89" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="25"/>
+      <c r="B89" s="28"/>
       <c r="C89" s="3">
         <v>90</v>
       </c>
       <c r="D89" s="12">
         <v>1167</v>
       </c>
-      <c r="E89" s="3"/>
+      <c r="E89" s="3">
+        <v>1250</v>
+      </c>
       <c r="F89" s="13">
         <f t="shared" si="3"/>
-        <v>-1167</v>
-      </c>
-      <c r="H89" s="19"/>
-      <c r="I89" s="19"/>
-      <c r="J89" s="19"/>
+        <v>83</v>
+      </c>
+      <c r="H89" s="22"/>
+      <c r="I89" s="22"/>
+      <c r="J89" s="22"/>
     </row>
     <row r="90" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="25"/>
+      <c r="B90" s="28"/>
       <c r="C90" s="3">
         <v>135</v>
       </c>
       <c r="D90" s="12">
         <v>1500</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3">
+        <v>1620</v>
+      </c>
       <c r="F90" s="13">
         <f t="shared" si="3"/>
-        <v>-1500</v>
-      </c>
-      <c r="H90" s="19"/>
-      <c r="I90" s="19"/>
-      <c r="J90" s="19"/>
+        <v>120</v>
+      </c>
+      <c r="H90" s="22"/>
+      <c r="I90" s="22"/>
+      <c r="J90" s="22"/>
     </row>
     <row r="91" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="26"/>
+      <c r="B91" s="29"/>
       <c r="C91" s="5">
         <v>180</v>
       </c>
       <c r="D91" s="14">
         <v>1833</v>
       </c>
-      <c r="E91" s="5"/>
-      <c r="F91" s="27">
+      <c r="E91" s="5">
+        <v>1940</v>
+      </c>
+      <c r="F91" s="15">
         <f t="shared" si="3"/>
-        <v>-1833</v>
-      </c>
-      <c r="H91" s="20"/>
-      <c r="I91" s="20"/>
-      <c r="J91" s="20"/>
+        <v>107</v>
+      </c>
+      <c r="H91" s="23"/>
+      <c r="I91" s="23"/>
+      <c r="J91" s="23"/>
     </row>
     <row r="92" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="24" t="s">
-        <v>16</v>
+      <c r="B92" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="C92" s="3">
         <v>0</v>
@@ -1844,86 +1966,102 @@
       <c r="D92" s="12">
         <v>500</v>
       </c>
-      <c r="E92" s="3"/>
-      <c r="F92" s="28">
+      <c r="E92" s="3">
+        <v>550</v>
+      </c>
+      <c r="F92" s="16">
         <f t="shared" si="3"/>
-        <v>-500</v>
-      </c>
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
-      <c r="J92" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="H92" s="21">
+        <v>1E-3</v>
+      </c>
+      <c r="I92" s="21">
+        <v>7.3639999999999999</v>
+      </c>
+      <c r="J92" s="21">
+        <v>548.74199999999996</v>
+      </c>
     </row>
     <row r="93" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="25"/>
+      <c r="B93" s="28"/>
       <c r="C93" s="3">
         <v>45</v>
       </c>
       <c r="D93" s="12">
         <v>833</v>
       </c>
-      <c r="E93" s="3"/>
+      <c r="E93" s="3">
+        <v>883</v>
+      </c>
       <c r="F93" s="13">
         <f t="shared" si="3"/>
-        <v>-833</v>
-      </c>
-      <c r="H93" s="19"/>
-      <c r="I93" s="19"/>
-      <c r="J93" s="19"/>
+        <v>50</v>
+      </c>
+      <c r="H93" s="22"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="22"/>
     </row>
     <row r="94" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="25"/>
+      <c r="B94" s="28"/>
       <c r="C94" s="3">
         <v>90</v>
       </c>
       <c r="D94" s="12">
         <v>1167</v>
       </c>
-      <c r="E94" s="3"/>
+      <c r="E94" s="3">
+        <v>1217</v>
+      </c>
       <c r="F94" s="13">
         <f t="shared" si="3"/>
-        <v>-1167</v>
-      </c>
-      <c r="H94" s="19"/>
-      <c r="I94" s="19"/>
-      <c r="J94" s="19"/>
+        <v>50</v>
+      </c>
+      <c r="H94" s="22"/>
+      <c r="I94" s="22"/>
+      <c r="J94" s="22"/>
     </row>
     <row r="95" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="25"/>
+      <c r="B95" s="28"/>
       <c r="C95" s="3">
         <v>135</v>
       </c>
       <c r="D95" s="12">
         <v>1500</v>
       </c>
-      <c r="E95" s="3"/>
+      <c r="E95" s="3">
+        <v>1580</v>
+      </c>
       <c r="F95" s="13">
         <f t="shared" si="3"/>
-        <v>-1500</v>
-      </c>
-      <c r="H95" s="19"/>
-      <c r="I95" s="19"/>
-      <c r="J95" s="19"/>
+        <v>80</v>
+      </c>
+      <c r="H95" s="22"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="22"/>
     </row>
     <row r="96" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="26"/>
+      <c r="B96" s="29"/>
       <c r="C96" s="5">
         <v>180</v>
       </c>
       <c r="D96" s="14">
         <v>1833</v>
       </c>
-      <c r="E96" s="5"/>
-      <c r="F96" s="27">
+      <c r="E96" s="5">
+        <v>1920</v>
+      </c>
+      <c r="F96" s="15">
         <f t="shared" si="3"/>
-        <v>-1833</v>
-      </c>
-      <c r="H96" s="20"/>
-      <c r="I96" s="20"/>
-      <c r="J96" s="20"/>
+        <v>87</v>
+      </c>
+      <c r="H96" s="23"/>
+      <c r="I96" s="23"/>
+      <c r="J96" s="23"/>
     </row>
     <row r="97" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="24" t="s">
-        <v>17</v>
+      <c r="B97" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="C97" s="3">
         <v>0</v>
@@ -1931,93 +2069,111 @@
       <c r="D97" s="12">
         <v>500</v>
       </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="28">
+      <c r="E97" s="3">
+        <v>560</v>
+      </c>
+      <c r="F97" s="16">
         <f t="shared" si="3"/>
-        <v>-500</v>
-      </c>
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
-      <c r="J97" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="H97" s="21">
+        <v>1E-3</v>
+      </c>
+      <c r="I97" s="21">
+        <v>7.1369999999999996</v>
+      </c>
+      <c r="J97" s="21">
+        <v>559.20000000000005</v>
+      </c>
     </row>
     <row r="98" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="25"/>
+      <c r="B98" s="28"/>
       <c r="C98" s="3">
         <v>45</v>
       </c>
       <c r="D98" s="12">
         <v>833</v>
       </c>
-      <c r="E98" s="3"/>
+      <c r="E98" s="3">
+        <v>883</v>
+      </c>
       <c r="F98" s="13">
         <f t="shared" si="3"/>
-        <v>-833</v>
-      </c>
-      <c r="H98" s="19"/>
-      <c r="I98" s="19"/>
-      <c r="J98" s="19"/>
+        <v>50</v>
+      </c>
+      <c r="H98" s="22"/>
+      <c r="I98" s="22"/>
+      <c r="J98" s="22"/>
     </row>
     <row r="99" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="25"/>
+      <c r="B99" s="28"/>
       <c r="C99" s="3">
         <v>90</v>
       </c>
       <c r="D99" s="12">
         <v>1167</v>
       </c>
-      <c r="E99" s="3"/>
+      <c r="E99" s="3">
+        <v>1210</v>
+      </c>
       <c r="F99" s="13">
         <f t="shared" si="3"/>
-        <v>-1167</v>
-      </c>
-      <c r="H99" s="19"/>
-      <c r="I99" s="19"/>
-      <c r="J99" s="19"/>
+        <v>43</v>
+      </c>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+      <c r="J99" s="22"/>
     </row>
     <row r="100" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="25"/>
+      <c r="B100" s="28"/>
       <c r="C100" s="3">
         <v>135</v>
       </c>
       <c r="D100" s="12">
         <v>1500</v>
       </c>
-      <c r="E100" s="3"/>
+      <c r="E100" s="3">
+        <v>1555</v>
+      </c>
       <c r="F100" s="13">
         <f t="shared" si="3"/>
-        <v>-1500</v>
-      </c>
-      <c r="H100" s="19"/>
-      <c r="I100" s="19"/>
-      <c r="J100" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="H100" s="22"/>
+      <c r="I100" s="22"/>
+      <c r="J100" s="22"/>
     </row>
     <row r="101" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="26"/>
+      <c r="B101" s="29"/>
       <c r="C101" s="5">
         <v>180</v>
       </c>
       <c r="D101" s="14">
         <v>1833</v>
       </c>
-      <c r="E101" s="5"/>
+      <c r="E101" s="5">
+        <v>1890</v>
+      </c>
       <c r="F101" s="13">
         <f t="shared" si="3"/>
-        <v>-1833</v>
-      </c>
-      <c r="H101" s="20"/>
-      <c r="I101" s="20"/>
-      <c r="J101" s="20"/>
+        <v>57</v>
+      </c>
+      <c r="H101" s="23"/>
+      <c r="I101" s="23"/>
+      <c r="J101" s="23"/>
     </row>
     <row r="102" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F102" s="29"/>
+      <c r="F102" s="17"/>
     </row>
     <row r="106" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="21"/>
-      <c r="C107" s="22"/>
-      <c r="D107" s="22"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="23"/>
+      <c r="B107" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" s="25"/>
+      <c r="D107" s="25"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="26"/>
       <c r="H107" s="9" t="s">
         <v>7</v>
       </c>
@@ -2049,8 +2205,8 @@
       </c>
     </row>
     <row r="109" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="24" t="s">
-        <v>15</v>
+      <c r="B109" s="27" t="s">
+        <v>28</v>
       </c>
       <c r="C109" s="3">
         <v>0</v>
@@ -2058,86 +2214,102 @@
       <c r="D109" s="12">
         <v>500</v>
       </c>
-      <c r="E109" s="3"/>
+      <c r="E109" s="3">
+        <v>620</v>
+      </c>
       <c r="F109" s="13">
         <f>E109-D109</f>
-        <v>-500</v>
-      </c>
-      <c r="H109" s="18"/>
-      <c r="I109" s="18"/>
-      <c r="J109" s="18"/>
+        <v>120</v>
+      </c>
+      <c r="H109" s="21">
+        <v>0</v>
+      </c>
+      <c r="I109" s="21">
+        <v>7.3840000000000003</v>
+      </c>
+      <c r="J109" s="21">
+        <v>614.85699999999997</v>
+      </c>
     </row>
     <row r="110" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="25"/>
+      <c r="B110" s="28"/>
       <c r="C110" s="3">
         <v>45</v>
       </c>
       <c r="D110" s="12">
         <v>833</v>
       </c>
-      <c r="E110" s="3"/>
+      <c r="E110" s="3">
+        <v>940</v>
+      </c>
       <c r="F110" s="13">
         <f t="shared" ref="F110:F123" si="4">E110-D110</f>
-        <v>-833</v>
-      </c>
-      <c r="H110" s="19"/>
-      <c r="I110" s="19"/>
-      <c r="J110" s="19"/>
+        <v>107</v>
+      </c>
+      <c r="H110" s="22"/>
+      <c r="I110" s="22"/>
+      <c r="J110" s="22"/>
     </row>
     <row r="111" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="25"/>
+      <c r="B111" s="28"/>
       <c r="C111" s="3">
         <v>90</v>
       </c>
       <c r="D111" s="12">
         <v>1167</v>
       </c>
-      <c r="E111" s="3"/>
+      <c r="E111" s="3">
+        <v>1280</v>
+      </c>
       <c r="F111" s="13">
         <f t="shared" si="4"/>
-        <v>-1167</v>
-      </c>
-      <c r="H111" s="19"/>
-      <c r="I111" s="19"/>
-      <c r="J111" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="H111" s="22"/>
+      <c r="I111" s="22"/>
+      <c r="J111" s="22"/>
     </row>
     <row r="112" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="25"/>
+      <c r="B112" s="28"/>
       <c r="C112" s="3">
         <v>135</v>
       </c>
       <c r="D112" s="12">
         <v>1500</v>
       </c>
-      <c r="E112" s="3"/>
+      <c r="E112" s="3">
+        <v>1640</v>
+      </c>
       <c r="F112" s="13">
         <f t="shared" si="4"/>
-        <v>-1500</v>
-      </c>
-      <c r="H112" s="19"/>
-      <c r="I112" s="19"/>
-      <c r="J112" s="19"/>
+        <v>140</v>
+      </c>
+      <c r="H112" s="22"/>
+      <c r="I112" s="22"/>
+      <c r="J112" s="22"/>
     </row>
     <row r="113" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="26"/>
+      <c r="B113" s="29"/>
       <c r="C113" s="5">
         <v>180</v>
       </c>
       <c r="D113" s="14">
         <v>1833</v>
       </c>
-      <c r="E113" s="5"/>
-      <c r="F113" s="27">
+      <c r="E113" s="5">
+        <v>1960</v>
+      </c>
+      <c r="F113" s="15">
         <f t="shared" si="4"/>
-        <v>-1833</v>
-      </c>
-      <c r="H113" s="20"/>
-      <c r="I113" s="20"/>
-      <c r="J113" s="20"/>
+        <v>127</v>
+      </c>
+      <c r="H113" s="23"/>
+      <c r="I113" s="23"/>
+      <c r="J113" s="23"/>
     </row>
     <row r="114" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="24" t="s">
-        <v>16</v>
+      <c r="B114" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="C114" s="3">
         <v>0</v>
@@ -2145,86 +2317,102 @@
       <c r="D114" s="12">
         <v>500</v>
       </c>
-      <c r="E114" s="3"/>
-      <c r="F114" s="28">
+      <c r="E114" s="3">
+        <v>630</v>
+      </c>
+      <c r="F114" s="16">
         <f t="shared" si="4"/>
-        <v>-500</v>
-      </c>
-      <c r="H114" s="18"/>
-      <c r="I114" s="18"/>
-      <c r="J114" s="18"/>
+        <v>130</v>
+      </c>
+      <c r="H114" s="21">
+        <v>0</v>
+      </c>
+      <c r="I114" s="21">
+        <v>7.7039999999999997</v>
+      </c>
+      <c r="J114" s="21">
+        <v>628.14200000000005</v>
+      </c>
     </row>
     <row r="115" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="25"/>
+      <c r="B115" s="28"/>
       <c r="C115" s="3">
         <v>45</v>
       </c>
       <c r="D115" s="12">
         <v>833</v>
       </c>
-      <c r="E115" s="3"/>
+      <c r="E115" s="3">
+        <v>970</v>
+      </c>
       <c r="F115" s="13">
         <f t="shared" si="4"/>
-        <v>-833</v>
-      </c>
-      <c r="H115" s="19"/>
-      <c r="I115" s="19"/>
-      <c r="J115" s="19"/>
+        <v>137</v>
+      </c>
+      <c r="H115" s="22"/>
+      <c r="I115" s="22"/>
+      <c r="J115" s="22"/>
     </row>
     <row r="116" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="25"/>
+      <c r="B116" s="28"/>
       <c r="C116" s="3">
         <v>90</v>
       </c>
       <c r="D116" s="12">
         <v>1167</v>
       </c>
-      <c r="E116" s="3"/>
+      <c r="E116" s="3">
+        <v>1315</v>
+      </c>
       <c r="F116" s="13">
         <f t="shared" si="4"/>
-        <v>-1167</v>
-      </c>
-      <c r="H116" s="19"/>
-      <c r="I116" s="19"/>
-      <c r="J116" s="19"/>
+        <v>148</v>
+      </c>
+      <c r="H116" s="22"/>
+      <c r="I116" s="22"/>
+      <c r="J116" s="22"/>
     </row>
     <row r="117" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="25"/>
+      <c r="B117" s="28"/>
       <c r="C117" s="3">
         <v>135</v>
       </c>
       <c r="D117" s="12">
         <v>1500</v>
       </c>
-      <c r="E117" s="3"/>
+      <c r="E117" s="3">
+        <v>1660</v>
+      </c>
       <c r="F117" s="13">
         <f t="shared" si="4"/>
-        <v>-1500</v>
-      </c>
-      <c r="H117" s="19"/>
-      <c r="I117" s="19"/>
-      <c r="J117" s="19"/>
+        <v>160</v>
+      </c>
+      <c r="H117" s="22"/>
+      <c r="I117" s="22"/>
+      <c r="J117" s="22"/>
     </row>
     <row r="118" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="26"/>
+      <c r="B118" s="29"/>
       <c r="C118" s="5">
         <v>180</v>
       </c>
       <c r="D118" s="14">
         <v>1833</v>
       </c>
-      <c r="E118" s="5"/>
-      <c r="F118" s="27">
+      <c r="E118" s="5">
+        <v>1990</v>
+      </c>
+      <c r="F118" s="15">
         <f t="shared" si="4"/>
-        <v>-1833</v>
-      </c>
-      <c r="H118" s="20"/>
-      <c r="I118" s="20"/>
-      <c r="J118" s="20"/>
+        <v>157</v>
+      </c>
+      <c r="H118" s="23"/>
+      <c r="I118" s="23"/>
+      <c r="J118" s="23"/>
     </row>
     <row r="119" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="24" t="s">
-        <v>17</v>
+      <c r="B119" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="C119" s="3">
         <v>0</v>
@@ -2232,85 +2420,101 @@
       <c r="D119" s="12">
         <v>500</v>
       </c>
-      <c r="E119" s="3"/>
-      <c r="F119" s="28">
+      <c r="E119" s="3">
+        <v>640</v>
+      </c>
+      <c r="F119" s="16">
         <f t="shared" si="4"/>
-        <v>-500</v>
-      </c>
-      <c r="H119" s="18"/>
-      <c r="I119" s="18"/>
-      <c r="J119" s="18"/>
+        <v>140</v>
+      </c>
+      <c r="H119" s="21">
+        <v>-1E-3</v>
+      </c>
+      <c r="I119" s="21">
+        <v>7.7649999999999997</v>
+      </c>
+      <c r="J119" s="21">
+        <v>634.28499999999997</v>
+      </c>
     </row>
     <row r="120" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="25"/>
+      <c r="B120" s="28"/>
       <c r="C120" s="3">
         <v>45</v>
       </c>
       <c r="D120" s="12">
         <v>833</v>
       </c>
-      <c r="E120" s="3"/>
+      <c r="E120" s="3">
+        <v>970</v>
+      </c>
       <c r="F120" s="13">
         <f t="shared" si="4"/>
-        <v>-833</v>
-      </c>
-      <c r="H120" s="19"/>
-      <c r="I120" s="19"/>
-      <c r="J120" s="19"/>
+        <v>137</v>
+      </c>
+      <c r="H120" s="22"/>
+      <c r="I120" s="22"/>
+      <c r="J120" s="22"/>
     </row>
     <row r="121" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="25"/>
+      <c r="B121" s="28"/>
       <c r="C121" s="3">
         <v>90</v>
       </c>
       <c r="D121" s="12">
         <v>1167</v>
       </c>
-      <c r="E121" s="3"/>
+      <c r="E121" s="3">
+        <v>1320</v>
+      </c>
       <c r="F121" s="13">
         <f t="shared" si="4"/>
-        <v>-1167</v>
-      </c>
-      <c r="H121" s="19"/>
-      <c r="I121" s="19"/>
-      <c r="J121" s="19"/>
+        <v>153</v>
+      </c>
+      <c r="H121" s="22"/>
+      <c r="I121" s="22"/>
+      <c r="J121" s="22"/>
     </row>
     <row r="122" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="25"/>
+      <c r="B122" s="28"/>
       <c r="C122" s="3">
         <v>135</v>
       </c>
       <c r="D122" s="12">
         <v>1500</v>
       </c>
-      <c r="E122" s="3"/>
+      <c r="E122" s="3">
+        <v>1670</v>
+      </c>
       <c r="F122" s="13">
         <f t="shared" si="4"/>
-        <v>-1500</v>
-      </c>
-      <c r="H122" s="19"/>
-      <c r="I122" s="19"/>
-      <c r="J122" s="19"/>
+        <v>170</v>
+      </c>
+      <c r="H122" s="22"/>
+      <c r="I122" s="22"/>
+      <c r="J122" s="22"/>
     </row>
     <row r="123" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="26"/>
+      <c r="B123" s="29"/>
       <c r="C123" s="5">
         <v>180</v>
       </c>
       <c r="D123" s="14">
         <v>1833</v>
       </c>
-      <c r="E123" s="5"/>
+      <c r="E123" s="5">
+        <v>1980</v>
+      </c>
       <c r="F123" s="13">
         <f t="shared" si="4"/>
-        <v>-1833</v>
-      </c>
-      <c r="H123" s="20"/>
-      <c r="I123" s="20"/>
-      <c r="J123" s="20"/>
+        <v>147</v>
+      </c>
+      <c r="H123" s="23"/>
+      <c r="I123" s="23"/>
+      <c r="J123" s="23"/>
     </row>
     <row r="124" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F124" s="29"/>
+      <c r="F124" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="67">

</xml_diff>

<commit_message>
calibration of new shoulder servo left
</commit_message>
<xml_diff>
--- a/save_coefficent/servo_DEG-PWM.xlsx
+++ b/save_coefficent/servo_DEG-PWM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\OneDrive\Desktop\1semestre\Bonzo - GoodBoy 0.0.0\botzo_v2s_github\calibrate_servos\save_coefficent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607681BE-8079-4854-BB4A-FC4EE6317877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5C59EC-6C21-41FF-95EF-15A37AB11563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>DATASHEET</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>TFR</t>
-  </si>
-  <si>
-    <t>TEST LEG</t>
   </si>
   <si>
     <t>FRONT RIGHT</t>
@@ -135,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -177,6 +174,20 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -364,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -421,6 +432,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,8 +657,8 @@
   </sheetPr>
   <dimension ref="B5:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="63" workbookViewId="0">
-      <selection activeCell="L95" sqref="L95"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="59" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -736,365 +752,38 @@
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
     </row>
-    <row r="18" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="H18" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="12">
-        <v>500</v>
-      </c>
-      <c r="E20" s="3">
-        <v>564</v>
-      </c>
-      <c r="F20" s="13">
-        <f>E20-D20</f>
-        <v>64</v>
-      </c>
-      <c r="H20" s="21">
-        <v>1E-3</v>
-      </c>
-      <c r="I20" s="21">
-        <v>7.2309999999999999</v>
-      </c>
-      <c r="J20" s="21">
-        <v>563.08500000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
-      <c r="C21" s="3">
-        <v>45</v>
-      </c>
-      <c r="D21" s="12">
-        <v>833</v>
-      </c>
-      <c r="E21" s="3">
-        <v>890</v>
-      </c>
-      <c r="F21" s="13">
-        <f t="shared" ref="F21:F34" si="0">E21-D21</f>
-        <v>57</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-    </row>
-    <row r="22" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
-      <c r="C22" s="3">
-        <v>90</v>
-      </c>
-      <c r="D22" s="12">
-        <v>1167</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1219</v>
-      </c>
-      <c r="F22" s="13">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-    </row>
-    <row r="23" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="28"/>
-      <c r="C23" s="3">
-        <v>135</v>
-      </c>
-      <c r="D23" s="12">
-        <v>1500</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1564</v>
-      </c>
-      <c r="F23" s="13">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-    </row>
-    <row r="24" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="29"/>
-      <c r="C24" s="5">
-        <v>180</v>
-      </c>
-      <c r="D24" s="14">
-        <v>1833</v>
-      </c>
-      <c r="E24" s="5">
-        <v>1897</v>
-      </c>
-      <c r="F24" s="15">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-    </row>
-    <row r="25" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="12">
-        <v>500</v>
-      </c>
-      <c r="E25" s="3">
-        <v>606</v>
-      </c>
-      <c r="F25" s="16">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="H25" s="21">
-        <v>0</v>
-      </c>
-      <c r="I25" s="21">
-        <v>7.3479999999999999</v>
-      </c>
-      <c r="J25" s="21">
-        <v>603.45699999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
-      <c r="C26" s="3">
-        <v>45</v>
-      </c>
-      <c r="D26" s="12">
-        <v>833</v>
-      </c>
-      <c r="E26" s="3">
-        <v>930</v>
-      </c>
-      <c r="F26" s="13">
-        <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-    </row>
-    <row r="27" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="28"/>
-      <c r="C27" s="3">
-        <v>90</v>
-      </c>
-      <c r="D27" s="12">
-        <v>1167</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1265</v>
-      </c>
-      <c r="F27" s="13">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-    </row>
-    <row r="28" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
-      <c r="C28" s="3">
-        <v>135</v>
-      </c>
-      <c r="D28" s="12">
-        <v>1500</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1606</v>
-      </c>
-      <c r="F28" s="13">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-    </row>
-    <row r="29" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="29"/>
-      <c r="C29" s="5">
-        <v>180</v>
-      </c>
-      <c r="D29" s="14">
-        <v>1833</v>
-      </c>
-      <c r="E29" s="5">
-        <v>1930</v>
-      </c>
-      <c r="F29" s="15">
-        <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-    </row>
-    <row r="30" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="12">
-        <v>500</v>
-      </c>
-      <c r="E30" s="3">
-        <v>555</v>
-      </c>
-      <c r="F30" s="16">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="H30" s="21">
-        <v>0</v>
-      </c>
-      <c r="I30" s="21">
-        <v>7.5759999999999996</v>
-      </c>
-      <c r="J30" s="21">
-        <v>554.28499999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="28"/>
-      <c r="C31" s="3">
-        <v>45</v>
-      </c>
-      <c r="D31" s="12">
-        <v>833</v>
-      </c>
-      <c r="E31" s="3">
-        <v>895</v>
-      </c>
-      <c r="F31" s="13">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-    </row>
-    <row r="32" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="28"/>
-      <c r="C32" s="3">
-        <v>90</v>
-      </c>
-      <c r="D32" s="12">
-        <v>1167</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1230</v>
-      </c>
-      <c r="F32" s="13">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-    </row>
-    <row r="33" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="28"/>
-      <c r="C33" s="3">
-        <v>135</v>
-      </c>
-      <c r="D33" s="12">
-        <v>1500</v>
-      </c>
-      <c r="E33" s="3">
-        <v>1580</v>
-      </c>
-      <c r="F33" s="13">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-    </row>
-    <row r="34" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="29"/>
-      <c r="C34" s="5">
-        <v>180</v>
-      </c>
-      <c r="D34" s="14">
-        <v>1833</v>
-      </c>
-      <c r="E34" s="5">
-        <v>1910</v>
-      </c>
-      <c r="F34" s="13">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-    </row>
-    <row r="35" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:10" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:10" ht="12.5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:10" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
-      <c r="F35" s="17"/>
-    </row>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
     </row>
     <row r="40" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
@@ -1169,7 +858,7 @@
         <v>933</v>
       </c>
       <c r="F43" s="13">
-        <f t="shared" ref="F43:F56" si="1">E43-D43</f>
+        <f t="shared" ref="F43:F56" si="0">E43-D43</f>
         <v>100</v>
       </c>
       <c r="H43" s="22"/>
@@ -1188,7 +877,7 @@
         <v>1267</v>
       </c>
       <c r="F44" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="H44" s="22"/>
@@ -1207,7 +896,7 @@
         <v>1620</v>
       </c>
       <c r="F45" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="H45" s="22"/>
@@ -1226,7 +915,7 @@
         <v>1940</v>
       </c>
       <c r="F46" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="H46" s="23"/>
@@ -1247,7 +936,7 @@
         <v>580</v>
       </c>
       <c r="F47" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="H47" s="21">
@@ -1272,7 +961,7 @@
         <v>920</v>
       </c>
       <c r="F48" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="H48" s="22"/>
@@ -1291,7 +980,7 @@
         <v>1260</v>
       </c>
       <c r="F49" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="H49" s="22"/>
@@ -1310,7 +999,7 @@
         <v>1610</v>
       </c>
       <c r="F50" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="H50" s="22"/>
@@ -1329,7 +1018,7 @@
         <v>1935</v>
       </c>
       <c r="F51" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
       <c r="H51" s="23"/>
@@ -1350,7 +1039,7 @@
         <v>620</v>
       </c>
       <c r="F52" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="H52" s="21">
@@ -1375,7 +1064,7 @@
         <v>950</v>
       </c>
       <c r="F53" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>117</v>
       </c>
       <c r="H53" s="22"/>
@@ -1394,7 +1083,7 @@
         <v>1278</v>
       </c>
       <c r="F54" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>111</v>
       </c>
       <c r="H54" s="22"/>
@@ -1413,7 +1102,7 @@
         <v>1630</v>
       </c>
       <c r="F55" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="H55" s="22"/>
@@ -1432,7 +1121,7 @@
         <v>1960</v>
       </c>
       <c r="F56" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="H56" s="23"/>
@@ -1465,13 +1154,13 @@
       <c r="D62" s="12"/>
     </row>
     <row r="63" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="26"/>
+      <c r="B63" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="32"/>
       <c r="H63" s="9" t="s">
         <v>7</v>
       </c>
@@ -1504,7 +1193,7 @@
     </row>
     <row r="65" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B65" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C65" s="3">
         <v>0</v>
@@ -1513,20 +1202,20 @@
         <v>500</v>
       </c>
       <c r="E65" s="3">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="F65" s="13">
         <f>E65-D65</f>
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H65" s="21">
         <v>0</v>
       </c>
       <c r="I65" s="21">
-        <v>7.4930000000000003</v>
+        <v>7.274</v>
       </c>
       <c r="J65" s="21">
-        <v>588.14200000000005</v>
+        <v>569.57100000000003</v>
       </c>
     </row>
     <row r="66" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -1538,11 +1227,11 @@
         <v>833</v>
       </c>
       <c r="E66" s="3">
-        <v>925</v>
+        <v>900</v>
       </c>
       <c r="F66" s="13">
-        <f t="shared" ref="F66:F79" si="2">E66-D66</f>
-        <v>92</v>
+        <f t="shared" ref="F66:F79" si="1">E66-D66</f>
+        <v>67</v>
       </c>
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
@@ -1557,11 +1246,11 @@
         <v>1167</v>
       </c>
       <c r="E67" s="3">
-        <v>1260</v>
+        <v>1225</v>
       </c>
       <c r="F67" s="13">
-        <f t="shared" si="2"/>
-        <v>93</v>
+        <f t="shared" si="1"/>
+        <v>58</v>
       </c>
       <c r="H67" s="22"/>
       <c r="I67" s="22"/>
@@ -1576,11 +1265,11 @@
         <v>1500</v>
       </c>
       <c r="E68" s="3">
-        <v>1620</v>
+        <v>1575</v>
       </c>
       <c r="F68" s="13">
-        <f t="shared" si="2"/>
-        <v>120</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="H68" s="22"/>
       <c r="I68" s="22"/>
@@ -1595,11 +1284,11 @@
         <v>1833</v>
       </c>
       <c r="E69" s="5">
-        <v>1950</v>
+        <v>1905</v>
       </c>
       <c r="F69" s="15">
-        <f t="shared" si="2"/>
-        <v>117</v>
+        <f t="shared" si="1"/>
+        <v>72</v>
       </c>
       <c r="H69" s="23"/>
       <c r="I69" s="23"/>
@@ -1607,7 +1296,7 @@
     </row>
     <row r="70" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C70" s="3">
         <v>0</v>
@@ -1619,7 +1308,7 @@
         <v>630</v>
       </c>
       <c r="F70" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="H70" s="21">
@@ -1644,7 +1333,7 @@
         <v>960</v>
       </c>
       <c r="F71" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="H71" s="22"/>
@@ -1663,7 +1352,7 @@
         <v>1310</v>
       </c>
       <c r="F72" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>143</v>
       </c>
       <c r="H72" s="22"/>
@@ -1682,7 +1371,7 @@
         <v>1670</v>
       </c>
       <c r="F73" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>170</v>
       </c>
       <c r="H73" s="22"/>
@@ -1701,7 +1390,7 @@
         <v>2000</v>
       </c>
       <c r="F74" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>167</v>
       </c>
       <c r="H74" s="23"/>
@@ -1710,7 +1399,7 @@
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C75" s="3">
         <v>0</v>
@@ -1722,7 +1411,7 @@
         <v>550</v>
       </c>
       <c r="F75" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="H75" s="21">
@@ -1747,7 +1436,7 @@
         <v>880</v>
       </c>
       <c r="F76" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="H76" s="22"/>
@@ -1766,7 +1455,7 @@
         <v>1205</v>
       </c>
       <c r="F77" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="H77" s="22"/>
@@ -1785,7 +1474,7 @@
         <v>1555</v>
       </c>
       <c r="F78" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="H78" s="22"/>
@@ -1804,7 +1493,7 @@
         <v>1890</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="H79" s="23"/>
@@ -1817,7 +1506,7 @@
     <row r="84" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B85" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="25"/>
@@ -1855,7 +1544,7 @@
     </row>
     <row r="87" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C87" s="3">
         <v>0</v>
@@ -1892,7 +1581,7 @@
         <v>910</v>
       </c>
       <c r="F88" s="13">
-        <f t="shared" ref="F88:F101" si="3">E88-D88</f>
+        <f t="shared" ref="F88:F101" si="2">E88-D88</f>
         <v>77</v>
       </c>
       <c r="H88" s="22"/>
@@ -1911,7 +1600,7 @@
         <v>1250</v>
       </c>
       <c r="F89" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="H89" s="22"/>
@@ -1930,7 +1619,7 @@
         <v>1620</v>
       </c>
       <c r="F90" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="H90" s="22"/>
@@ -1949,7 +1638,7 @@
         <v>1940</v>
       </c>
       <c r="F91" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="H91" s="23"/>
@@ -1958,7 +1647,7 @@
     </row>
     <row r="92" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C92" s="3">
         <v>0</v>
@@ -1970,7 +1659,7 @@
         <v>550</v>
       </c>
       <c r="F92" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="H92" s="21">
@@ -1995,7 +1684,7 @@
         <v>883</v>
       </c>
       <c r="F93" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="H93" s="22"/>
@@ -2014,7 +1703,7 @@
         <v>1217</v>
       </c>
       <c r="F94" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="H94" s="22"/>
@@ -2033,7 +1722,7 @@
         <v>1580</v>
       </c>
       <c r="F95" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="H95" s="22"/>
@@ -2052,7 +1741,7 @@
         <v>1920</v>
       </c>
       <c r="F96" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="H96" s="23"/>
@@ -2061,7 +1750,7 @@
     </row>
     <row r="97" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C97" s="3">
         <v>0</v>
@@ -2073,7 +1762,7 @@
         <v>560</v>
       </c>
       <c r="F97" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="H97" s="21">
@@ -2098,7 +1787,7 @@
         <v>883</v>
       </c>
       <c r="F98" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="H98" s="22"/>
@@ -2117,7 +1806,7 @@
         <v>1210</v>
       </c>
       <c r="F99" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="H99" s="22"/>
@@ -2136,7 +1825,7 @@
         <v>1555</v>
       </c>
       <c r="F100" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="H100" s="22"/>
@@ -2155,7 +1844,7 @@
         <v>1890</v>
       </c>
       <c r="F101" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="H101" s="23"/>
@@ -2168,7 +1857,7 @@
     <row r="106" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C107" s="25"/>
       <c r="D107" s="25"/>
@@ -2206,7 +1895,7 @@
     </row>
     <row r="109" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C109" s="3">
         <v>0</v>
@@ -2243,7 +1932,7 @@
         <v>940</v>
       </c>
       <c r="F110" s="13">
-        <f t="shared" ref="F110:F123" si="4">E110-D110</f>
+        <f t="shared" ref="F110:F123" si="3">E110-D110</f>
         <v>107</v>
       </c>
       <c r="H110" s="22"/>
@@ -2262,7 +1951,7 @@
         <v>1280</v>
       </c>
       <c r="F111" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="H111" s="22"/>
@@ -2281,7 +1970,7 @@
         <v>1640</v>
       </c>
       <c r="F112" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="H112" s="22"/>
@@ -2300,7 +1989,7 @@
         <v>1960</v>
       </c>
       <c r="F113" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="H113" s="23"/>
@@ -2309,7 +1998,7 @@
     </row>
     <row r="114" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C114" s="3">
         <v>0</v>
@@ -2321,7 +2010,7 @@
         <v>630</v>
       </c>
       <c r="F114" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="H114" s="21">
@@ -2346,7 +2035,7 @@
         <v>970</v>
       </c>
       <c r="F115" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>137</v>
       </c>
       <c r="H115" s="22"/>
@@ -2365,7 +2054,7 @@
         <v>1315</v>
       </c>
       <c r="F116" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>148</v>
       </c>
       <c r="H116" s="22"/>
@@ -2384,7 +2073,7 @@
         <v>1660</v>
       </c>
       <c r="F117" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="H117" s="22"/>
@@ -2403,7 +2092,7 @@
         <v>1990</v>
       </c>
       <c r="F118" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>157</v>
       </c>
       <c r="H118" s="23"/>
@@ -2412,7 +2101,7 @@
     </row>
     <row r="119" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C119" s="3">
         <v>0</v>
@@ -2424,7 +2113,7 @@
         <v>640</v>
       </c>
       <c r="F119" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="H119" s="21">
@@ -2449,7 +2138,7 @@
         <v>970</v>
       </c>
       <c r="F120" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>137</v>
       </c>
       <c r="H120" s="22"/>
@@ -2468,7 +2157,7 @@
         <v>1320</v>
       </c>
       <c r="F121" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>153</v>
       </c>
       <c r="H121" s="22"/>
@@ -2487,7 +2176,7 @@
         <v>1670</v>
       </c>
       <c r="F122" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
       <c r="H122" s="22"/>
@@ -2506,7 +2195,7 @@
         <v>1980</v>
       </c>
       <c r="F123" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>147</v>
       </c>
       <c r="H123" s="23"/>
@@ -2517,74 +2206,61 @@
       <c r="F124" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="54">
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="H119:H123"/>
+    <mergeCell ref="I119:I123"/>
+    <mergeCell ref="J119:J123"/>
+    <mergeCell ref="B109:B113"/>
+    <mergeCell ref="H109:H113"/>
+    <mergeCell ref="I109:I113"/>
+    <mergeCell ref="J109:J113"/>
     <mergeCell ref="B114:B118"/>
     <mergeCell ref="H114:H118"/>
     <mergeCell ref="I114:I118"/>
     <mergeCell ref="J114:J118"/>
-    <mergeCell ref="B119:B123"/>
-    <mergeCell ref="H119:H123"/>
-    <mergeCell ref="I119:I123"/>
-    <mergeCell ref="J119:J123"/>
+    <mergeCell ref="B97:B101"/>
+    <mergeCell ref="H97:H101"/>
+    <mergeCell ref="I97:I101"/>
+    <mergeCell ref="J97:J101"/>
     <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B109:B113"/>
-    <mergeCell ref="H109:H113"/>
-    <mergeCell ref="I109:I113"/>
-    <mergeCell ref="J109:J113"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="H87:H91"/>
+    <mergeCell ref="I87:I91"/>
+    <mergeCell ref="J87:J91"/>
     <mergeCell ref="B92:B96"/>
     <mergeCell ref="H92:H96"/>
     <mergeCell ref="I92:I96"/>
     <mergeCell ref="J92:J96"/>
-    <mergeCell ref="B97:B101"/>
-    <mergeCell ref="H97:H101"/>
-    <mergeCell ref="I97:I101"/>
-    <mergeCell ref="J97:J101"/>
+    <mergeCell ref="B75:B79"/>
+    <mergeCell ref="H75:H79"/>
+    <mergeCell ref="I75:I79"/>
+    <mergeCell ref="J75:J79"/>
     <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="H87:H91"/>
-    <mergeCell ref="I87:I91"/>
-    <mergeCell ref="J87:J91"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="H65:H69"/>
+    <mergeCell ref="I65:I69"/>
+    <mergeCell ref="J65:J69"/>
     <mergeCell ref="B70:B74"/>
     <mergeCell ref="H70:H74"/>
     <mergeCell ref="I70:I74"/>
     <mergeCell ref="J70:J74"/>
-    <mergeCell ref="B75:B79"/>
-    <mergeCell ref="H75:H79"/>
-    <mergeCell ref="I75:I79"/>
-    <mergeCell ref="J75:J79"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="H52:H56"/>
+    <mergeCell ref="I52:I56"/>
+    <mergeCell ref="J52:J56"/>
     <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="H65:H69"/>
-    <mergeCell ref="I65:I69"/>
-    <mergeCell ref="J65:J69"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="H42:H46"/>
+    <mergeCell ref="I42:I46"/>
+    <mergeCell ref="J42:J46"/>
     <mergeCell ref="B47:B51"/>
     <mergeCell ref="H47:H51"/>
     <mergeCell ref="I47:I51"/>
     <mergeCell ref="J47:J51"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="H52:H56"/>
-    <mergeCell ref="I52:I56"/>
-    <mergeCell ref="J52:J56"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="H42:H46"/>
-    <mergeCell ref="I42:I46"/>
-    <mergeCell ref="J42:J46"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H14:I15"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="H25:H29"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="J30:J34"/>
-    <mergeCell ref="I30:I34"/>
-    <mergeCell ref="J25:J29"/>
-    <mergeCell ref="I25:I29"/>
-    <mergeCell ref="J20:J24"/>
-    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="B40:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>